<commit_message>
Work in progress -> Check for overlap
</commit_message>
<xml_diff>
--- a/res/shm-copy.xlsx
+++ b/res/shm-copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\msc\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5072F45-4EFE-4D4A-9773-83278E7720EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA24549-4106-4DCD-BE7F-5E7794D49236}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4080" yWindow="1845" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{5B3A39F9-A350-47F0-9C4B-CDFDDFCA56E6}"/>
   </bookViews>
@@ -5516,7 +5516,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -5553,7 +5553,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -5579,19 +5579,13 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="34925" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -6236,7 +6230,7 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -9681,7 +9675,7 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="342">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -9692,7 +9686,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -9705,7 +9699,7 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
@@ -9722,7 +9716,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -9738,7 +9732,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -9782,35 +9776,45 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="34925" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -9822,29 +9826,31 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -9948,8 +9954,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -10039,20 +10051,20 @@
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -10065,17 +10077,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -10107,7 +10108,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -10116,13 +10117,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -10176,8 +10178,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -17020,7 +17028,7 @@
   <dimension ref="A1:D200"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="D177" sqref="D177"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>